<commit_message>
align opti with new reference
</commit_message>
<xml_diff>
--- a/projects/alignment-opti/plots_pub/align-res_no-masking.xlsx
+++ b/projects/alignment-opti/plots_pub/align-res_no-masking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>sample_name_unique</t>
   </si>
@@ -73,9 +73,6 @@
     <t>40h_1</t>
   </si>
   <si>
-    <t>40h_NoOx_1</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
   </si>
   <si>
     <t>S8</t>
-  </si>
-  <si>
-    <t>S9</t>
   </si>
 </sst>
 </file>
@@ -458,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,16 +501,16 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>99.3180056185308</v>
+        <v>99.32416523349828</v>
       </c>
       <c r="D2">
-        <v>69.90607535604831</v>
+        <v>68.28859604845688</v>
       </c>
       <c r="E2">
-        <v>10.1529655669731</v>
+        <v>10.2277725699452</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -527,16 +521,16 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>98.8751834929778</v>
+        <v>99.37021207967101</v>
       </c>
       <c r="D3">
-        <v>69.6167557166136</v>
+        <v>68.51697066256951</v>
       </c>
       <c r="E3">
-        <v>12.981849037929</v>
+        <v>10.2433500050944</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -547,16 +541,16 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>99.3651316997824</v>
+        <v>98.7402667566686</v>
       </c>
       <c r="D4">
-        <v>70.1084981664504</v>
+        <v>66.60510628094494</v>
       </c>
       <c r="E4">
-        <v>10.1739234715085</v>
+        <v>13.57176929140085</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -567,16 +561,16 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>99.16890254209819</v>
+        <v>99.31888229250808</v>
       </c>
       <c r="D5">
-        <v>69.8442298129322</v>
+        <v>68.24273052095465</v>
       </c>
       <c r="E5">
-        <v>13.5412661550371</v>
+        <v>9.346941192727559</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -587,16 +581,16 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>98.7344434397346</v>
+        <v>98.83333010442296</v>
       </c>
       <c r="D6">
-        <v>68.31180029311641</v>
+        <v>68.06867810909776</v>
       </c>
       <c r="E6">
-        <v>13.5097558766768</v>
+        <v>11.17891278609345</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -607,16 +601,16 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>99.3126099412366</v>
+        <v>98.84969293180292</v>
       </c>
       <c r="D7">
-        <v>70.05562452027409</v>
+        <v>68.19941794255345</v>
       </c>
       <c r="E7">
-        <v>9.301234731685129</v>
+        <v>9.39398540638576</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -627,16 +621,16 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>99.0918296957377</v>
+        <v>99.15328876853674</v>
       </c>
       <c r="D8">
-        <v>69.8584479448127</v>
+        <v>68.30072837970894</v>
       </c>
       <c r="E8">
-        <v>11.9391784463809</v>
+        <v>15.52677299785912</v>
       </c>
       <c r="L8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -647,36 +641,16 @@
         <v>18</v>
       </c>
       <c r="C9">
-        <v>98.82515455688529</v>
+        <v>98.64836954674628</v>
       </c>
       <c r="D9">
-        <v>69.8987823693512</v>
+        <v>66.08044396034251</v>
       </c>
       <c r="E9">
-        <v>11.1066892248216</v>
+        <v>14.15203097545656</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>98.8452956303345</v>
-      </c>
-      <c r="D10">
-        <v>69.8735469285148</v>
-      </c>
-      <c r="E10">
-        <v>9.344536113782461</v>
-      </c>
-      <c r="L10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>